<commit_message>
Implemented basic task list and timer using default SQLite database instead of Supabase .
</commit_message>
<xml_diff>
--- a/documentation/keywords.xlsx
+++ b/documentation/keywords.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\project\StudyMate\documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C84AFA-8EFA-4121-AA81-0A5AC60B6477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9463" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,15 +24,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>binding</t>
+  </si>
+  <si>
+    <t>AuthActivity.kt</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6.8"/>
+      <color rgb="FF871094"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +72,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +356,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>